<commit_message>
Unit test for category and changed session notes
</commit_message>
<xml_diff>
--- a/ExploratorySessionNotes/CategorySession.xlsx
+++ b/ExploratorySessionNotes/CategorySession.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ECSE-428\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ECSE-429\ecse429-project-partA\ExploratorySessionNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64E52B2B-9007-4577-A48E-2F13223504B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26253C34-E999-4849-A40A-DF3C50A57308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="154">
   <si>
     <t>Method</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>14.png</t>
-  </si>
-  <si>
-    <t>supporting PUT as an HTTP request method for a general resource family as opposed to a particular instance of a resource does not make sense</t>
   </si>
   <si>
     <t>15.png</t>
@@ -577,6 +574,15 @@
   </si>
   <si>
     <t>5.    What happens if you attempt to DELETE /categories/{id} for a category ID that doesn't exist? Does the API return a 404 Not Found, or does it behave differently, such as returning 200 OK without any changes?</t>
+  </si>
+  <si>
+    <t>Reference of File Created as part of exploratory testing:</t>
+  </si>
+  <si>
+    <t>CategorySession.xlsx</t>
+  </si>
+  <si>
+    <t>supporting PUT as an HTTP request method for a general resource family can make sense if it creates a particular instance of a resource if one does not exist</t>
   </si>
 </sst>
 </file>
@@ -775,7 +781,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -873,6 +879,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -1279,16 +1288,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB764FF"/>
+          <bgColor rgb="FFB764FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB764FF"/>
-          <bgColor rgb="FFB764FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1314,6 +1323,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB764FF"/>
+          <bgColor rgb="FFB764FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
@@ -1346,8 +1363,32 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB764FF"/>
-          <bgColor rgb="FFB764FF"/>
+          <fgColor rgb="FFFF005B"/>
+          <bgColor rgb="FFFF005B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1365,32 +1406,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF005B"/>
-          <bgColor rgb="FFFF005B"/>
+          <fgColor rgb="FFB764FF"/>
+          <bgColor rgb="FFB764FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1399,14 +1416,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB764FF"/>
-          <bgColor rgb="FFB764FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1623,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="51" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
@@ -1785,7 +1794,7 @@
         <v>51</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>52</v>
@@ -1887,7 +1896,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="13" t="s">
@@ -1942,7 +1951,7 @@
         <v>72</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>73</v>
@@ -2026,7 +2035,7 @@
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="62.4">
+    <row r="16" spans="1:9" ht="62.4" customHeight="1">
       <c r="A16" s="24" t="s">
         <v>36</v>
       </c>
@@ -2046,10 +2055,10 @@
         <v>56</v>
       </c>
       <c r="G16" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>85</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>86</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -2064,25 +2073,25 @@
         <v>8</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G17" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="28" t="s">
         <v>88</v>
-      </c>
-      <c r="H17" s="28" t="s">
-        <v>89</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="15.6">
       <c r="A18" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>10</v>
@@ -2091,23 +2100,23 @@
         <v>5</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="62.4">
       <c r="A19" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>13</v>
@@ -2128,13 +2137,13 @@
         <v>83</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="31.2">
       <c r="A20" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>7</v>
@@ -2143,7 +2152,7 @@
         <v>8</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>23</v>
@@ -2152,16 +2161,16 @@
         <v>56</v>
       </c>
       <c r="G20" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="28" t="s">
         <v>97</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>98</v>
       </c>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="31.2">
       <c r="A21" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>11</v>
@@ -2170,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>23</v>
@@ -2179,16 +2188,16 @@
         <v>56</v>
       </c>
       <c r="G21" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="28" t="s">
         <v>100</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>101</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="31.2">
       <c r="A22" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>12</v>
@@ -2197,7 +2206,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>6</v>
@@ -2206,16 +2215,16 @@
         <v>51</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="46.8">
       <c r="A23" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>39</v>
@@ -2224,7 +2233,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>6</v>
@@ -2233,16 +2242,16 @@
         <v>41</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="A24" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>4</v>
@@ -2251,23 +2260,23 @@
         <v>5</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" ht="15.6">
       <c r="A25" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>11</v>
@@ -2276,23 +2285,23 @@
         <v>5</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" ht="15.6">
       <c r="A26" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>10</v>
@@ -2301,23 +2310,23 @@
         <v>5</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G26" s="33"/>
       <c r="H26" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" ht="46.8">
       <c r="A27" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>39</v>
@@ -2326,7 +2335,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>6</v>
@@ -2335,16 +2344,16 @@
         <v>41</v>
       </c>
       <c r="G27" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>4</v>
@@ -2353,23 +2362,23 @@
         <v>5</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" ht="15.6">
       <c r="A29" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>11</v>
@@ -2378,23 +2387,23 @@
         <v>5</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G29" s="29"/>
       <c r="H29" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="15.6">
       <c r="A30" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>4</v>
@@ -2403,23 +2412,23 @@
         <v>5</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G30" s="23"/>
       <c r="H30" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>4</v>
@@ -2428,17 +2437,17 @@
         <v>5</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G31" s="23"/>
       <c r="H31" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -4651,43 +4660,43 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B1:B2 B4:B10">
-    <cfRule type="cellIs" dxfId="58" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="215" operator="equal">
+      <formula>"HEAD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="214" operator="equal">
       <formula>"PATCH"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="215" operator="equal">
-      <formula>"HEAD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="216" operator="equal">
-      <formula>"OPTIONS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="217" operator="equal">
-      <formula>"DELETE"</formula>
+    <cfRule type="cellIs" dxfId="56" priority="220" operator="equal">
+      <formula>"PUT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="219" operator="equal">
+      <formula>"GET"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="54" priority="218" operator="equal">
       <formula>"POST"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="219" operator="equal">
-      <formula>"GET"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="220" operator="equal">
-      <formula>"PUT"</formula>
+    <cfRule type="cellIs" dxfId="53" priority="217" operator="equal">
+      <formula>"DELETE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="216" operator="equal">
+      <formula>"OPTIONS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B22">
-    <cfRule type="cellIs" dxfId="51" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="78" operator="equal">
+      <formula>"HEAD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="79" operator="equal">
+      <formula>"OPTIONS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="80" operator="equal">
+      <formula>"DELETE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="81" operator="equal">
+      <formula>"POST"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="77" operator="equal">
       <formula>"PATCH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="78" operator="equal">
-      <formula>"HEAD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="79" operator="equal">
-      <formula>"OPTIONS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="80" operator="equal">
-      <formula>"DELETE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="81" operator="equal">
-      <formula>"POST"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="46" priority="82" operator="equal">
       <formula>"GET"</formula>
@@ -4697,11 +4706,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="cellIs" dxfId="44" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="37" operator="equal">
+      <formula>"HEAD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
       <formula>"PATCH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="37" operator="equal">
-      <formula>"HEAD"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
       <formula>"OPTIONS"</formula>
@@ -4897,10 +4906,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1"/>
@@ -5106,7 +5115,7 @@
     <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -5128,7 +5137,7 @@
     <row r="19" spans="1:8" ht="15" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -5140,7 +5149,7 @@
     <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -5152,7 +5161,7 @@
     <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -5164,7 +5173,7 @@
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -5176,7 +5185,7 @@
     <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -5197,7 +5206,7 @@
     <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -5231,7 +5240,7 @@
     <row r="28" spans="1:8" ht="82.2" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -5252,7 +5261,7 @@
     <row r="30" spans="1:8" ht="124.8">
       <c r="A30" s="2"/>
       <c r="B30" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -5275,30 +5284,38 @@
     <row r="33" spans="1:2" ht="15" customHeight="1">
       <c r="A33" s="2"/>
       <c r="B33" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1">
       <c r="A34" s="2"/>
       <c r="B34" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1">
       <c r="A35" s="4"/>
       <c r="B35" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
       <c r="A36" s="4"/>
       <c r="B36" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1">
       <c r="B37" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="31.2">
+      <c r="A40" s="39" t="s">
         <v>151</v>
+      </c>
+      <c r="B40" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -5311,14 +5328,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="4a222ce7-d792-41a4-94c0-7b8554ef6272" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5327,7 +5336,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006ACCA6F238C8B94FAD54C37A52440078" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f0299a2a93b4df195ab26d9284b966fb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77b571ba-450d-45b4-9c3d-d33771cba36b" xmlns:ns4="4a222ce7-d792-41a4-94c0-7b8554ef6272" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f25a8803bdda655fcd6b8f32e045d113" ns3:_="" ns4:_="">
     <xsd:import namespace="77b571ba-450d-45b4-9c3d-d33771cba36b"/>
@@ -5554,24 +5563,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AFA97AD-3091-43E0-9236-A183989BAB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="77b571ba-450d-45b4-9c3d-d33771cba36b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="4a222ce7-d792-41a4-94c0-7b8554ef6272"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="4a222ce7-d792-41a4-94c0-7b8554ef6272" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B4E5F-5944-4700-9348-D8CEACE8A5D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5579,7 +5579,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B170E91-EE3E-4E89-AF87-4B9B3E3A462F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5596,4 +5596,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AFA97AD-3091-43E0-9236-A183989BAB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="77b571ba-450d-45b4-9c3d-d33771cba36b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4a222ce7-d792-41a4-94c0-7b8554ef6272"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>